<commit_message>
Update default replacements sheet.
</commit_message>
<xml_diff>
--- a/xlsx/hfc_replacements.xlsx
+++ b/xlsx/hfc_replacements.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\high-frequency-checks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\high-frequency-checks\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,21 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>id</t>
   </si>
   <si>
     <t>enumerator</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>drop</t>
   </si>
   <si>
     <t>newvalue</t>
@@ -47,11 +38,17 @@
   <si>
     <t>variable</t>
   </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>selectmultiple</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -83,15 +80,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -120,6 +142,75 @@
           <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -138,20 +229,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -204,7 +301,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
-            <a:t>readreplace</a:t>
+            <a:t>ipacheckreadreplace</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
@@ -288,20 +385,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -360,20 +463,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -431,20 +540,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -493,77 +608,6 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
             <a:t>This column specifies the new value that will be placed in the survey data set.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8915400" y="5381624"/>
-          <a:ext cx="3667125" cy="828675"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FF0000"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>drop</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies whether the given id observation should be dropped (caution this should only be used for duplicates or incomplete/invalid interviews).</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -650,6 +694,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -685,6 +746,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -837,63 +915,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:9">
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:H1048576">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>$A1&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>A$1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:I1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$A1&lt;&gt;""</formula>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>I$1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>